<commit_message>
working on isolating to diff file
</commit_message>
<xml_diff>
--- a/ARCC/ Code/ex.xlsx
+++ b/ARCC/ Code/ex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,23 +467,29 @@
       <c r="H1" s="1" t="inlineStr"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Fair Value</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr"/>
-      <c r="K1" s="1" t="inlineStr">
+          <t>Fair  Value</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Fair  Value  Per Unit</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr"/>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Percentage  of Net  Assets</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AGILE Fund I, LLC (7)(9)</t>
+          <t>AGILE  Fund I, LLC (7)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -493,7 +499,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Member interest (0.50% interest)</t>
+          <t>Member interest (0.50%  interest)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -508,29 +514,35 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>217</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BB&amp;T Capital Partners/Windsor Mezzanine Fund, LLC (6)(9)</t>
+          <t>BB&amp;T  Capital Partners/Windsor Mezzanine Fund, LLC (6)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Investment company</t>
+          <t>Investment partnership</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Member interest (32.59% interest)</t>
+          <t>Member interest (32.59%  interest)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -541,25 +553,27 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10108</t>
+          <t>12877</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>13976</t>
+          <t>15190</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Carador PLC (6)(8)(9)(16)</t>
+          <t>Callidus  Debt Partners CDO Fund I, Ltd. (8)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -569,114 +583,144 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ordinary shares (7,110,525 shares)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Class C notes  ($18,800 par due 12/2013)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4.59%</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>12/15/2006</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9033</t>
+          <t>2518</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>6613</t>
+          <t>1448</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CIC Flex, LP (9)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Investment partnership</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Limited partnership units (0.94 unit)</t>
+          <t>Class D notes  ($9,400 par due 12/2013)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>9/7/2007</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2553</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>(13)(16)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Covestia Capital Partners, LP (9)</t>
+          <t>Callidus  Debt Partners CLO Fund III, Ltd. (8)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Investment partnership</t>
+          <t>Investment company</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Limited partnership interest (47.00% interest)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>Preferred shares (23,600,000  shares )</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9.05%</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>6/17/2008</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1059</t>
+          <t>4753</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1041</t>
+          <t>6874</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dynamic India Fund IV, LLC (9)</t>
+          <t>Callidus  Debt Partners CLO Fund IV, Ltd. (8)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -686,10 +730,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Member interest (5.44% interest)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Class D notes  ($3,000 par due 4/2020)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4.84% (Libor +  4.55%/Q)</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>4/1/2010</t>
@@ -697,147 +745,195 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4822</t>
+          <t>1789</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4728</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.58</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Firstlight Financial Corporation (6)(9)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Investment company</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Senior subordinated loan ($73,993 par due 12/2016)</t>
+          <t>Subordinated notes  ($17,500 par due 4/2020)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.00% PIK</t>
+          <t>14.03%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>12/31/2006</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>73708</t>
+          <t>7216</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>56670</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>(4)</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
+          <t>10285</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Callidus  Debt Partners CLO Fund V, Ltd. (8)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Common stock (10,000 shares)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>Subordinated notes  ($14,150 par due 11/2020)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>19.70%</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>12/31/2006</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>8692</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>11096</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Callidus  Debt Partners CLO Fund VI, Ltd. (8)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Common stock (30,000 shares)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>Class D notes  ($9,000 par due 10/2021)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6.29% (Libor +  6.00%/Q)</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>12/31/2006</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>30000</t>
+          <t>3962</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>4241</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>HCI Equity, LLC (7)(8)(9)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Investment company</t>
-        </is>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Member interest (100% interest)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>Subordinated notes  ($25,500 par due 10/2021)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>18.39%</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>4/1/2010</t>
@@ -845,64 +941,88 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>808</t>
+          <t>11050</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>943</t>
+          <t>17101</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Imperial Capital Private Opportunities, LP (6)(9)</t>
+          <t>Callidus  Debt Partners CLO Fund VII, Ltd. (8)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Investment partnership</t>
+          <t>Investment company</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Limited partnership interest (80% interest)</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>Subordinated notes  ($28,000 par due 1/2021)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>13.27%</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5/10/2007</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>6643</t>
+          <t>10374</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>5300</t>
+          <t>15080</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ivy Hill Middle Market Credit Fund, Ltd. (7)(8)(9)</t>
+          <t>Callidus  MAPS CLO Fund I LLC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -912,75 +1032,95 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Class B deferrable interest notes ($40,000 par due 11/2018)</t>
+          <t>Class E notes  ($17,000 par due 12/2017)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.25% (Libor + 6.00%/Q)</t>
+          <t>5.80% (Libor +  5.53%/Q)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11/20/2007</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>40000</t>
+          <t>11679</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>37600</t>
+          <t>11244</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Subordinated notes ($16 par due 11/2018)</t>
+          <t>Subordinated Notes  ($47,900 par due 12/2017)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>15.50%</t>
+          <t>9.18%</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>11/20/2007</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>15515</t>
+          <t>13419</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>17946</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Knightsbridge CLO 2007-1 Ltd. (7)(8)(9)</t>
+          <t>Callidus  MAPS CLO Fund II, Ltd.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -990,153 +1130,185 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Class E notes ($20,350 par due 1/2022)</t>
+          <t>Class D notes  ($7,700 par due 7/2022)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>9.30% (Libor + 9.00%/Q)</t>
+          <t>4.54% (Libor +  4.25%/Q)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3/24/2010</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>14852</t>
+          <t>3324</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>17324</t>
+          <t>4049</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Knightsbridge CLO 2008-1 Ltd. (7)(8)(9)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Investment company</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Class C notes ($14,400 par due 6/2018)</t>
+          <t>Subordinated notes  ($17,900 par due 7/2022)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>7.81% (Libor + 7.50%/Q)</t>
+          <t>19.30%</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>3/24/2010</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>14400</t>
+          <t>8977</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>14400</t>
+          <t>12906</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.72</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Catterton  Partners VI, L.P.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Investment partnership</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Class D notes ($9,000 par due 6/2018)</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>8.81% (Libor + 8.50%/Q)</t>
-        </is>
-      </c>
+          <t>Limited partnership  interest (0.50% interest)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>3/24/2010</t>
+          <t>4/1/2010</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>9000</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>9000</t>
+          <t>2226</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CIC  Flex, LP (9)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Investment partnership</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Class E notes ($14,850 par due 6/2018)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>5.31% (Libor + 5.00%/Q)</t>
-        </is>
-      </c>
+          <t>Limited partnership  units (0.94 unit)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3/24/2010</t>
+          <t>9/7/2007</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>13596</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>13634</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kodiak Funding, LP (9)</t>
+          <t>Cortec  Group Fund IV, L.P.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1146,7 +1318,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Limited partnership interest (1.52% interest)</t>
+          <t>Limited partnership  interest (2.53% interest)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1157,17 +1329,771 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>905</t>
+          <t>4628</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>788</t>
+          <t>4355</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Covestia  Capital Partners, LP (9)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Investment partnership</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Limited partnership  interest (47.00% interest)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>6/17/2008</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1059</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>982</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Dryden  XVIII Leveraged Loan 2007 Limited (8)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Class B notes  ($9,000 par due 10/2019)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>4.79% (Libor +  4.50%/Q)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>3753</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3562</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Subordinated notes  ($21,164 par due 10/2019)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>22.03%</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>12715</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>16486</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Dynamic  India Fund IV</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Member interest (5.44%  interest)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>4822</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>4822</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Fidus  Mezzanine Capital, L.P.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Investment partnership</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Limited partnership  interest (29.12% interest)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>9206</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>9588</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Firstlight  Financial Corporation (6)(9)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Senior subordinated loan  ($73,625 par due 12/2016)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1.00% PIK</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>12/31/2006</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>73433</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>47857</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>(4)(16)</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Common stock (10,000  shares )</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>12/31/2006</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Common stock (30,000  shares )</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>12/31/2006</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>30000</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>HCI Private  Equity Managers, LP (7) (8)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Member interest (100%  interest)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>973</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Ivy  Hill Middle Market Credit Fund, Ltd. (7)(8)(9)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Class B deferrable  interest notes ($40,000 par due 11/2018)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6.48% (Libor +  6.00%/Q)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>11/20/2007</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>15351</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>14737</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Subordinated notes  ($15,351 par due 11/2018)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>15.50%</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>11/20/2007</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>37200</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Knightsbridge  CLO 2007-1 Ltd. (7)(8)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Class E notes  ($20,350 par due 1/2022)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>9.29% (Libor +  9.00%/Q)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>3/24/2010</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>14852</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>11296</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Knightsbridge  CLO 2008-1 Ltd. (7)(8)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Investment company</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Class C notes  ($14,400 par due 6/2018)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7.79% (Libor +  7.50%/Q)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>3/24/2010</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>14400</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>14400</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Class D notes  ($9,000 par due 6/2018)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>8.79% (Libor +  8.50%/Q)</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>3/24/2010</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Class E notes  ($14,850 par due 6/2018)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>5.29% (Libor +  5.00%/Q)</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>3/24/2010</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>13596</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>9914</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>(16)</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Kodiak  Fund LP</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Investment partnership</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Limited partnership  interest (1.52% interest)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4/1/2010</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>932</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>